<commit_message>
modify sop, add support for section, add support for increment/decrement on while
</commit_message>
<xml_diff>
--- a/output/sop2-extracted.xlsx
+++ b/output/sop2-extracted.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="69">
   <si>
     <t>STEP NUMBER</t>
   </si>
@@ -25,6 +25,15 @@
     <t>VALUE</t>
   </si>
   <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>section</t>
+  </si>
+  <si>
+    <t>Structure Preparation</t>
+  </si>
+  <si>
     <t>examined organisms</t>
   </si>
   <si>
@@ -142,7 +151,7 @@
     <t>target criteria</t>
   </si>
   <si>
-    <t>&lt;=5  Å</t>
+    <t>lte 5  Å</t>
   </si>
   <si>
     <t>optimization</t>
@@ -169,6 +178,18 @@
     <t>flow compared value</t>
   </si>
   <si>
+    <t>flow operation</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>flow magnitude</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>(minimization)  target</t>
   </si>
   <si>
@@ -200,18 +221,6 @@
   </si>
   <si>
     <t>[1-7]</t>
-  </si>
-  <si>
-    <t>flow operation</t>
-  </si>
-  <si>
-    <t>+</t>
-  </si>
-  <si>
-    <t>flow magnitude</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
 </sst>
 </file>
@@ -543,7 +552,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C74"/>
+  <dimension ref="A1:C77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -561,25 +570,25 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -587,10 +596,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -598,10 +607,10 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -609,10 +618,10 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -620,21 +629,21 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -642,10 +651,10 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -653,10 +662,10 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -664,21 +673,21 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -686,10 +695,10 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -697,10 +706,10 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -708,10 +717,10 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -719,10 +728,10 @@
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -730,10 +739,10 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -741,21 +750,21 @@
         <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -763,10 +772,10 @@
         <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -774,10 +783,10 @@
         <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C21" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -785,10 +794,10 @@
         <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -796,10 +805,10 @@
         <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C23" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -807,10 +816,10 @@
         <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C24" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -818,10 +827,10 @@
         <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C25" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -829,21 +838,21 @@
         <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C26" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="C27" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -851,10 +860,10 @@
         <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C28" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -862,10 +871,10 @@
         <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C29" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -873,10 +882,10 @@
         <v>6</v>
       </c>
       <c r="B30" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C30" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -884,10 +893,10 @@
         <v>6</v>
       </c>
       <c r="B31" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C31" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -895,10 +904,10 @@
         <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="C32" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -906,10 +915,10 @@
         <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C33" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -917,10 +926,10 @@
         <v>6</v>
       </c>
       <c r="B34" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="C34" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -928,10 +937,10 @@
         <v>6</v>
       </c>
       <c r="B35" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C35" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -939,43 +948,43 @@
         <v>6</v>
       </c>
       <c r="B36" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="C36" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B37" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C37" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B38" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C38" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B39" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="C39" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -983,10 +992,10 @@
         <v>7</v>
       </c>
       <c r="B40" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="C40" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -994,10 +1003,10 @@
         <v>7</v>
       </c>
       <c r="B41" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="C41" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1005,10 +1014,10 @@
         <v>7</v>
       </c>
       <c r="B42" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C42" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1016,10 +1025,10 @@
         <v>7</v>
       </c>
       <c r="B43" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="C43" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1027,10 +1036,10 @@
         <v>7</v>
       </c>
       <c r="B44" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="C44" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1038,10 +1047,10 @@
         <v>7</v>
       </c>
       <c r="B45" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C45" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1049,43 +1058,43 @@
         <v>7</v>
       </c>
       <c r="B46" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C46" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B47" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C47" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B48" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C48" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B49" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="C49" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1093,10 +1102,10 @@
         <v>8</v>
       </c>
       <c r="B50" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="C50" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1104,10 +1113,10 @@
         <v>8</v>
       </c>
       <c r="B51" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="C51" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1115,10 +1124,10 @@
         <v>8</v>
       </c>
       <c r="B52" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C52" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1126,10 +1135,10 @@
         <v>8</v>
       </c>
       <c r="B53" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="C53" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1137,10 +1146,10 @@
         <v>8</v>
       </c>
       <c r="B54" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="C54" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1148,10 +1157,10 @@
         <v>8</v>
       </c>
       <c r="B55" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C55" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1159,43 +1168,43 @@
         <v>8</v>
       </c>
       <c r="B56" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C56" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B57" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C57" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B58" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C58" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B59" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="C59" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1203,10 +1212,10 @@
         <v>9</v>
       </c>
       <c r="B60" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C60" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1214,10 +1223,10 @@
         <v>9</v>
       </c>
       <c r="B61" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C61" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1225,10 +1234,10 @@
         <v>9</v>
       </c>
       <c r="B62" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C62" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1236,43 +1245,43 @@
         <v>9</v>
       </c>
       <c r="B63" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C63" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B64" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C64" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B65" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C65" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B66" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="C66" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1280,10 +1289,10 @@
         <v>10</v>
       </c>
       <c r="B67" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="C67" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1291,10 +1300,10 @@
         <v>10</v>
       </c>
       <c r="B68" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="C68" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1302,10 +1311,10 @@
         <v>10</v>
       </c>
       <c r="B69" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="C69" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1313,10 +1322,10 @@
         <v>10</v>
       </c>
       <c r="B70" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="C70" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1324,10 +1333,10 @@
         <v>10</v>
       </c>
       <c r="B71" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="C71" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1335,10 +1344,10 @@
         <v>10</v>
       </c>
       <c r="B72" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="C72" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1346,10 +1355,10 @@
         <v>10</v>
       </c>
       <c r="B73" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C73" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -1357,10 +1366,43 @@
         <v>10</v>
       </c>
       <c r="B74" t="s">
+        <v>42</v>
+      </c>
+      <c r="C74" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75">
+        <v>10</v>
+      </c>
+      <c r="B75" t="s">
         <v>44</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C75" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76">
+        <v>10</v>
+      </c>
+      <c r="B76" t="s">
+        <v>40</v>
+      </c>
+      <c r="C76" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77">
+        <v>10</v>
+      </c>
+      <c r="B77" t="s">
+        <v>47</v>
+      </c>
+      <c r="C77" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
support start/end extraction for range within ifelse and for
</commit_message>
<xml_diff>
--- a/output/sop2-extracted.xlsx
+++ b/output/sop2-extracted.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="60">
   <si>
     <t>STEP NUMBER</t>
   </si>
@@ -25,15 +25,6 @@
     <t>VALUE</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>section</t>
-  </si>
-  <si>
-    <t>Structure Preparation</t>
-  </si>
-  <si>
     <t>examined organisms</t>
   </si>
   <si>
@@ -118,64 +109,79 @@
     <t>BioLuminate package</t>
   </si>
   <si>
+    <t>operation</t>
+  </si>
+  <si>
+    <t>energy minimization</t>
+  </si>
+  <si>
+    <t>(minimization) target</t>
+  </si>
+  <si>
+    <t>receptor residue</t>
+  </si>
+  <si>
+    <t>target criteria</t>
+  </si>
+  <si>
+    <t>lte 5  Å</t>
+  </si>
+  <si>
+    <t>optimization</t>
+  </si>
+  <si>
+    <t>(optimization) target</t>
+  </si>
+  <si>
+    <t>side chain rotamers</t>
+  </si>
+  <si>
+    <t>(minimization)  target</t>
+  </si>
+  <si>
     <t>step type</t>
   </si>
   <si>
+    <t>conditional</t>
+  </si>
+  <si>
+    <t>flow type</t>
+  </si>
+  <si>
+    <t>else if</t>
+  </si>
+  <si>
+    <t>flow parameter</t>
+  </si>
+  <si>
+    <t>pH</t>
+  </si>
+  <si>
+    <t>flow logical parameter</t>
+  </si>
+  <si>
+    <t>between</t>
+  </si>
+  <si>
+    <t>flow range</t>
+  </si>
+  <si>
+    <t>[8-12]</t>
+  </si>
+  <si>
+    <t>start iteration value</t>
+  </si>
+  <si>
+    <t>end iteration value</t>
+  </si>
+  <si>
     <t>iteration</t>
   </si>
   <si>
-    <t>flow type</t>
-  </si>
-  <si>
-    <t>for each</t>
-  </si>
-  <si>
-    <t>flow parameter</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> generated pose</t>
-  </si>
-  <si>
-    <t>operation</t>
-  </si>
-  <si>
-    <t>energy minimization</t>
-  </si>
-  <si>
-    <t>(minimization) target</t>
-  </si>
-  <si>
-    <t>receptor residue</t>
-  </si>
-  <si>
-    <t>target criteria</t>
-  </si>
-  <si>
-    <t>lte 5  Å</t>
-  </si>
-  <si>
-    <t>optimization</t>
-  </si>
-  <si>
-    <t>(optimization) target</t>
-  </si>
-  <si>
-    <t>side chain rotamers</t>
-  </si>
-  <si>
-    <t>while</t>
-  </si>
-  <si>
-    <t>pH</t>
-  </si>
-  <si>
-    <t>flow logical parameter</t>
-  </si>
-  <si>
-    <t>lte</t>
-  </si>
-  <si>
-    <t>flow compared value</t>
+    <t>for</t>
+  </si>
+  <si>
+    <t>[1-7]</t>
   </si>
   <si>
     <t>flow operation</t>
@@ -188,39 +194,6 @@
   </si>
   <si>
     <t>1</t>
-  </si>
-  <si>
-    <t>(minimization)  target</t>
-  </si>
-  <si>
-    <t>conditional</t>
-  </si>
-  <si>
-    <t>if</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7 </t>
-  </si>
-  <si>
-    <t>else if</t>
-  </si>
-  <si>
-    <t>between</t>
-  </si>
-  <si>
-    <t>[8-12]</t>
-  </si>
-  <si>
-    <t>else</t>
-  </si>
-  <si>
-    <t>for</t>
-  </si>
-  <si>
-    <t>flow range</t>
-  </si>
-  <si>
-    <t>[1-7]</t>
   </si>
 </sst>
 </file>
@@ -552,7 +525,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C77"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -570,25 +543,25 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -596,10 +569,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -607,10 +580,10 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
         <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -618,10 +591,10 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
         <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -629,21 +602,21 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
         <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -651,10 +624,10 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -662,10 +635,10 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
         <v>18</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -673,21 +646,21 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
         <v>20</v>
-      </c>
-      <c r="C11" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -695,10 +668,10 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -706,10 +679,10 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
         <v>25</v>
-      </c>
-      <c r="C14" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -717,10 +690,10 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" t="s">
         <v>27</v>
-      </c>
-      <c r="C15" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -728,10 +701,10 @@
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -739,10 +712,10 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -750,21 +723,21 @@
         <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="C19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -772,10 +745,10 @@
         <v>5</v>
       </c>
       <c r="B20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" t="s">
         <v>34</v>
-      </c>
-      <c r="C20" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -783,10 +756,10 @@
         <v>5</v>
       </c>
       <c r="B21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" t="s">
         <v>36</v>
-      </c>
-      <c r="C21" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -794,10 +767,10 @@
         <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C22" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -805,54 +778,54 @@
         <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C23" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C24" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C25" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C26" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="C27" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -860,549 +833,395 @@
         <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C28" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C29" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B30" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C30" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B31" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="C31" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="C32" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B33" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="C33" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B34" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="C34" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B35" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C35" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B36" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C36" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B37" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C37" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C38" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B39" t="s">
-        <v>47</v>
-      </c>
-      <c r="C39" t="s">
-        <v>48</v>
+        <v>51</v>
+      </c>
+      <c r="C39">
+        <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>34</v>
-      </c>
-      <c r="C40" t="s">
-        <v>59</v>
+        <v>52</v>
+      </c>
+      <c r="C40">
+        <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B41" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C41" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B42" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C42" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B43" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="C43" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B44" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="C44" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B45" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C45" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B46" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C46" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B47" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C47" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B48" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C48" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B49" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="C49" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B50" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C50" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B51" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C51" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B52" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C52" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B53" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C53" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B54" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C54" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B55" t="s">
-        <v>40</v>
-      </c>
-      <c r="C55" t="s">
-        <v>41</v>
+        <v>51</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B56" t="s">
-        <v>42</v>
-      </c>
-      <c r="C56" t="s">
-        <v>43</v>
+        <v>52</v>
+      </c>
+      <c r="C56">
+        <v>7</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B57" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C57" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B58" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="C58" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B59" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="C59" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B60" t="s">
+        <v>33</v>
+      </c>
+      <c r="C60" t="s">
         <v>34</v>
-      </c>
-      <c r="C60" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B61" t="s">
+        <v>35</v>
+      </c>
+      <c r="C61" t="s">
         <v>36</v>
-      </c>
-      <c r="C61" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B62" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C62" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B63" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C63" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64">
-        <v>9</v>
-      </c>
-      <c r="B64" t="s">
-        <v>44</v>
-      </c>
-      <c r="C64" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65">
-        <v>9</v>
-      </c>
-      <c r="B65" t="s">
-        <v>40</v>
-      </c>
-      <c r="C65" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66">
-        <v>9</v>
-      </c>
-      <c r="B66" t="s">
-        <v>47</v>
-      </c>
-      <c r="C66" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67">
-        <v>10</v>
-      </c>
-      <c r="B67" t="s">
-        <v>34</v>
-      </c>
-      <c r="C67" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68">
-        <v>10</v>
-      </c>
-      <c r="B68" t="s">
-        <v>36</v>
-      </c>
-      <c r="C68" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69">
-        <v>10</v>
-      </c>
-      <c r="B69" t="s">
-        <v>38</v>
-      </c>
-      <c r="C69" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="A70">
-        <v>10</v>
-      </c>
-      <c r="B70" t="s">
-        <v>67</v>
-      </c>
-      <c r="C70" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="A71">
-        <v>10</v>
-      </c>
-      <c r="B71" t="s">
-        <v>54</v>
-      </c>
-      <c r="C71" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72">
-        <v>10</v>
-      </c>
-      <c r="B72" t="s">
-        <v>56</v>
-      </c>
-      <c r="C72" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="A73">
-        <v>10</v>
-      </c>
-      <c r="B73" t="s">
-        <v>40</v>
-      </c>
-      <c r="C73" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74">
-        <v>10</v>
-      </c>
-      <c r="B74" t="s">
-        <v>42</v>
-      </c>
-      <c r="C74" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75">
-        <v>10</v>
-      </c>
-      <c r="B75" t="s">
-        <v>44</v>
-      </c>
-      <c r="C75" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
-      <c r="A76">
-        <v>10</v>
-      </c>
-      <c r="B76" t="s">
-        <v>40</v>
-      </c>
-      <c r="C76" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="A77">
-        <v>10</v>
-      </c>
-      <c r="B77" t="s">
-        <v>47</v>
-      </c>
-      <c r="C77" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bugfixes for flow control
</commit_message>
<xml_diff>
--- a/output/sop2-extracted.xlsx
+++ b/output/sop2-extracted.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="71">
   <si>
     <t>STEP NUMBER</t>
   </si>
@@ -25,6 +25,15 @@
     <t>VALUE</t>
   </si>
   <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>section</t>
+  </si>
+  <si>
+    <t>Structure Preparation</t>
+  </si>
+  <si>
     <t>examined organisms</t>
   </si>
   <si>
@@ -109,6 +118,24 @@
     <t>BioLuminate package</t>
   </si>
   <si>
+    <t>step type</t>
+  </si>
+  <si>
+    <t>iteration</t>
+  </si>
+  <si>
+    <t>flow type</t>
+  </si>
+  <si>
+    <t>for each</t>
+  </si>
+  <si>
+    <t>flow parameter</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> generated pose</t>
+  </si>
+  <si>
     <t>operation</t>
   </si>
   <si>
@@ -136,30 +163,48 @@
     <t>side chain rotamers</t>
   </si>
   <si>
+    <t>while</t>
+  </si>
+  <si>
+    <t>pH</t>
+  </si>
+  <si>
+    <t>flow logical parameter</t>
+  </si>
+  <si>
+    <t>lte</t>
+  </si>
+  <si>
+    <t>flow compared value</t>
+  </si>
+  <si>
+    <t>flow operation</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>flow magnitude</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>(minimization)  target</t>
   </si>
   <si>
-    <t>step type</t>
-  </si>
-  <si>
     <t>conditional</t>
   </si>
   <si>
-    <t>flow type</t>
+    <t>if</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 </t>
   </si>
   <si>
     <t>else if</t>
   </si>
   <si>
-    <t>flow parameter</t>
-  </si>
-  <si>
-    <t>pH</t>
-  </si>
-  <si>
-    <t>flow logical parameter</t>
-  </si>
-  <si>
     <t>between</t>
   </si>
   <si>
@@ -175,25 +220,13 @@
     <t>end iteration value</t>
   </si>
   <si>
-    <t>iteration</t>
+    <t>else</t>
   </si>
   <si>
     <t>for</t>
   </si>
   <si>
     <t>[1-7]</t>
-  </si>
-  <si>
-    <t>flow operation</t>
-  </si>
-  <si>
-    <t>+</t>
-  </si>
-  <si>
-    <t>flow magnitude</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
 </sst>
 </file>
@@ -525,7 +558,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C63"/>
+  <dimension ref="A1:C81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -543,25 +576,25 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -569,10 +602,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -580,10 +613,10 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -591,10 +624,10 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -602,21 +635,21 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -624,10 +657,10 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -635,10 +668,10 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -646,21 +679,21 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -668,10 +701,10 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -679,10 +712,10 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -690,10 +723,10 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -701,10 +734,10 @@
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -712,10 +745,10 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -723,21 +756,21 @@
         <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -745,10 +778,10 @@
         <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -756,10 +789,10 @@
         <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C21" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -767,10 +800,10 @@
         <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C22" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -778,54 +811,54 @@
         <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C23" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C24" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C25" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C26" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="C27" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -833,395 +866,593 @@
         <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C28" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C29" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B30" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C30" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B31" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="C31" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="C32" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="C33" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B34" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="C34" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B35" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C35" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B36" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="C36" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B37" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C37" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B38" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C38" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B39" t="s">
-        <v>51</v>
-      </c>
-      <c r="C39">
-        <v>8</v>
+        <v>47</v>
+      </c>
+      <c r="C39" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B40" t="s">
-        <v>52</v>
-      </c>
-      <c r="C40">
-        <v>12</v>
+        <v>34</v>
+      </c>
+      <c r="C40" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B41" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C41" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B42" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C42" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B43" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="C43" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B44" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="C44" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B45" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C45" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B46" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C46" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B47" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="C47" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B48" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C48" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B49" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="C49" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B50" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C50" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B51" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C51" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B52" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C52" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B53" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C53" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B54" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="C54" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B55" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="C55">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B56" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="C56">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B57" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="C57" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B58" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="C58" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B59" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C59" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B60" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C60" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B61" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="C61" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B62" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C62" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63">
+        <v>9</v>
+      </c>
+      <c r="B63" t="s">
+        <v>36</v>
+      </c>
+      <c r="C63" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64">
+        <v>9</v>
+      </c>
+      <c r="B64" t="s">
+        <v>40</v>
+      </c>
+      <c r="C64" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65">
+        <v>9</v>
+      </c>
+      <c r="B65" t="s">
+        <v>42</v>
+      </c>
+      <c r="C65" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66">
+        <v>9</v>
+      </c>
+      <c r="B66" t="s">
+        <v>44</v>
+      </c>
+      <c r="C66" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67">
+        <v>9</v>
+      </c>
+      <c r="B67" t="s">
+        <v>40</v>
+      </c>
+      <c r="C67" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68">
+        <v>9</v>
+      </c>
+      <c r="B68" t="s">
+        <v>47</v>
+      </c>
+      <c r="C68" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69">
         <v>10</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B69" t="s">
+        <v>34</v>
+      </c>
+      <c r="C69" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70">
+        <v>10</v>
+      </c>
+      <c r="B70" t="s">
+        <v>36</v>
+      </c>
+      <c r="C70" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71">
+        <v>10</v>
+      </c>
+      <c r="B71" t="s">
         <v>38</v>
       </c>
-      <c r="C63" t="s">
-        <v>39</v>
+      <c r="C71" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72">
+        <v>10</v>
+      </c>
+      <c r="B72" t="s">
+        <v>64</v>
+      </c>
+      <c r="C72" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73">
+        <v>10</v>
+      </c>
+      <c r="B73" t="s">
+        <v>66</v>
+      </c>
+      <c r="C73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74">
+        <v>10</v>
+      </c>
+      <c r="B74" t="s">
+        <v>67</v>
+      </c>
+      <c r="C74">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75">
+        <v>10</v>
+      </c>
+      <c r="B75" t="s">
+        <v>54</v>
+      </c>
+      <c r="C75" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76">
+        <v>10</v>
+      </c>
+      <c r="B76" t="s">
+        <v>56</v>
+      </c>
+      <c r="C76" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77">
+        <v>10</v>
+      </c>
+      <c r="B77" t="s">
+        <v>40</v>
+      </c>
+      <c r="C77" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78">
+        <v>10</v>
+      </c>
+      <c r="B78" t="s">
+        <v>42</v>
+      </c>
+      <c r="C78" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79">
+        <v>10</v>
+      </c>
+      <c r="B79" t="s">
+        <v>44</v>
+      </c>
+      <c r="C79" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80">
+        <v>10</v>
+      </c>
+      <c r="B80" t="s">
+        <v>40</v>
+      </c>
+      <c r="C80" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81">
+        <v>10</v>
+      </c>
+      <c r="B81" t="s">
+        <v>47</v>
+      </c>
+      <c r="C81" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
comment parsing - not yet serialized
</commit_message>
<xml_diff>
--- a/output/sop2-extracted.xlsx
+++ b/output/sop2-extracted.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="69">
   <si>
     <t>STEP NUMBER</t>
   </si>
@@ -142,7 +142,7 @@
     <t>energy minimization</t>
   </si>
   <si>
-    <t>(minimization) target</t>
+    <t>target</t>
   </si>
   <si>
     <t>receptor residue</t>
@@ -157,9 +157,6 @@
     <t>optimization</t>
   </si>
   <si>
-    <t>(optimization) target</t>
-  </si>
-  <si>
     <t>side chain rotamers</t>
   </si>
   <si>
@@ -188,9 +185,6 @@
   </si>
   <si>
     <t>1</t>
-  </si>
-  <si>
-    <t>(minimization)  target</t>
   </si>
   <si>
     <t>conditional</t>
@@ -855,10 +849,10 @@
         <v>5</v>
       </c>
       <c r="B27" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" t="s">
         <v>47</v>
-      </c>
-      <c r="C27" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -880,7 +874,7 @@
         <v>36</v>
       </c>
       <c r="C29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -891,7 +885,7 @@
         <v>38</v>
       </c>
       <c r="C30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -899,10 +893,10 @@
         <v>6</v>
       </c>
       <c r="B31" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" t="s">
         <v>51</v>
-      </c>
-      <c r="C31" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -910,7 +904,7 @@
         <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C32" t="s">
         <v>14</v>
@@ -921,10 +915,10 @@
         <v>6</v>
       </c>
       <c r="B33" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33" t="s">
         <v>54</v>
-      </c>
-      <c r="C33" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -932,10 +926,10 @@
         <v>6</v>
       </c>
       <c r="B34" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" t="s">
         <v>56</v>
-      </c>
-      <c r="C34" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -954,7 +948,7 @@
         <v>6</v>
       </c>
       <c r="B36" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="C36" t="s">
         <v>43</v>
@@ -987,10 +981,10 @@
         <v>6</v>
       </c>
       <c r="B39" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" t="s">
         <v>47</v>
-      </c>
-      <c r="C39" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1001,7 +995,7 @@
         <v>34</v>
       </c>
       <c r="C40" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1012,7 +1006,7 @@
         <v>36</v>
       </c>
       <c r="C41" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1023,7 +1017,7 @@
         <v>38</v>
       </c>
       <c r="C42" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1031,10 +1025,10 @@
         <v>7</v>
       </c>
       <c r="B43" t="s">
+        <v>50</v>
+      </c>
+      <c r="C43" t="s">
         <v>51</v>
-      </c>
-      <c r="C43" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1042,10 +1036,10 @@
         <v>7</v>
       </c>
       <c r="B44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C44" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1097,10 +1091,10 @@
         <v>7</v>
       </c>
       <c r="B49" t="s">
+        <v>42</v>
+      </c>
+      <c r="C49" t="s">
         <v>47</v>
-      </c>
-      <c r="C49" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1111,7 +1105,7 @@
         <v>34</v>
       </c>
       <c r="C50" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1122,7 +1116,7 @@
         <v>36</v>
       </c>
       <c r="C51" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1133,7 +1127,7 @@
         <v>38</v>
       </c>
       <c r="C52" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1141,10 +1135,10 @@
         <v>8</v>
       </c>
       <c r="B53" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C53" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1152,10 +1146,10 @@
         <v>8</v>
       </c>
       <c r="B54" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C54" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1163,7 +1157,7 @@
         <v>8</v>
       </c>
       <c r="B55" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C55">
         <v>8</v>
@@ -1174,7 +1168,7 @@
         <v>8</v>
       </c>
       <c r="B56" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C56">
         <v>12</v>
@@ -1229,10 +1223,10 @@
         <v>8</v>
       </c>
       <c r="B61" t="s">
+        <v>42</v>
+      </c>
+      <c r="C61" t="s">
         <v>47</v>
-      </c>
-      <c r="C61" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1243,7 +1237,7 @@
         <v>34</v>
       </c>
       <c r="C62" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1254,7 +1248,7 @@
         <v>36</v>
       </c>
       <c r="C63" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1306,10 +1300,10 @@
         <v>9</v>
       </c>
       <c r="B68" t="s">
+        <v>42</v>
+      </c>
+      <c r="C68" t="s">
         <v>47</v>
-      </c>
-      <c r="C68" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1331,7 +1325,7 @@
         <v>36</v>
       </c>
       <c r="C70" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1342,7 +1336,7 @@
         <v>38</v>
       </c>
       <c r="C71" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1350,10 +1344,10 @@
         <v>10</v>
       </c>
       <c r="B72" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C72" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1361,7 +1355,7 @@
         <v>10</v>
       </c>
       <c r="B73" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C73">
         <v>1</v>
@@ -1372,7 +1366,7 @@
         <v>10</v>
       </c>
       <c r="B74" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C74">
         <v>7</v>
@@ -1383,10 +1377,10 @@
         <v>10</v>
       </c>
       <c r="B75" t="s">
+        <v>53</v>
+      </c>
+      <c r="C75" t="s">
         <v>54</v>
-      </c>
-      <c r="C75" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -1394,10 +1388,10 @@
         <v>10</v>
       </c>
       <c r="B76" t="s">
+        <v>55</v>
+      </c>
+      <c r="C76" t="s">
         <v>56</v>
-      </c>
-      <c r="C76" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -1449,10 +1443,10 @@
         <v>10</v>
       </c>
       <c r="B81" t="s">
+        <v>42</v>
+      </c>
+      <c r="C81" t="s">
         <v>47</v>
-      </c>
-      <c r="C81" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>